<commit_message>
add for another PC
</commit_message>
<xml_diff>
--- a/Tugboat Problem V3-Demo.xlsx
+++ b/Tugboat Problem V3-Demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\Aj Kanchana Projects\TugBoat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77CC276-CBCC-4E13-9FCA-190AFA5A0233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0615ABC6-670C-4FBD-A95A-EFA4697D72CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="5" r:id="rId1"/>
@@ -784,16 +784,16 @@
     <t>2025-01-17 18:00:00</t>
   </si>
   <si>
-    <t>2025-01-22 18:00:00</t>
-  </si>
-  <si>
-    <t>2025-01-19 08:00:00</t>
-  </si>
-  <si>
-    <t>2025-01-23 18:00:00</t>
-  </si>
-  <si>
     <t>o4</t>
+  </si>
+  <si>
+    <t>2025-01-24 18:00:00</t>
+  </si>
+  <si>
+    <t>2025-01-21 08:00:00</t>
+  </si>
+  <si>
+    <t>2025-01-26 18:00:00</t>
   </si>
 </sst>
 </file>
@@ -1162,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W993"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1404,7 +1404,7 @@
         <v>233</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I4" s="1">
         <v>2000</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>193</v>
@@ -1466,10 +1466,10 @@
         <v>20000</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I5" s="1">
         <v>400</v>
@@ -2571,7 +2571,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>7</v>
@@ -8370,7 +8370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>